<commit_message>
Cập nhật timeline tuần 1
</commit_message>
<xml_diff>
--- a/FIleSumary/FileSumaryDoAn.xlsx
+++ b/FIleSumary/FileSumaryDoAn.xlsx
@@ -137,8 +137,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -408,7 +408,7 @@
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -419,21 +419,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,8 +440,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -461,19 +457,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -793,7 +793,7 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -814,30 +814,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="24">
         <f ca="1">I2-L2</f>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -860,24 +860,24 @@
       </c>
       <c r="L2" s="11">
         <f ca="1">TODAY()</f>
-        <v>43933</v>
+        <v>43934</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="15" t="s">
         <v>18</v>
       </c>
@@ -886,21 +886,21 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="J5" s="25" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="J5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="24"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
@@ -913,619 +913,631 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="23" t="s">
         <v>35</v>
       </c>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="32">
+      <c r="A8" s="33">
         <v>1</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37" t="s">
+      <c r="E8" s="27">
+        <v>43939</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="32"/>
     </row>
     <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37" t="s">
+      <c r="E9" s="27">
+        <v>43939</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="32"/>
     </row>
     <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37" t="s">
+      <c r="E10" s="27">
+        <v>43939</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="32"/>
     </row>
     <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37" t="s">
+      <c r="E11" s="27">
+        <v>43939</v>
+      </c>
+      <c r="F11" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37" t="s">
+      <c r="E12" s="27">
+        <v>43939</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="32"/>
     </row>
     <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34" t="s">
+      <c r="A13" s="33"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37" t="s">
+      <c r="E13" s="27">
+        <v>43939</v>
+      </c>
+      <c r="F13" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="32"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="32">
+      <c r="A14" s="33">
         <v>2</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="30"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="32"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="30"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="32"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="30"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="32"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="30"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="32"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="30"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="32"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="30"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="32"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="30"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="32"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="30"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="32"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="30"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="32"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="30"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="32"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="30"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="32"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="30"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="32"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="30"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="32"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="30"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="32"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="30"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="32"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="30"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="32"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="30"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="32"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="30"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="32"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="30"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="32"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="30"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="32"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="30"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="32"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="30"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="32"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="30"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="32"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="30"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="32"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="30"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="32"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
-      <c r="L39" s="30"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="32"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="30"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="32"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="38"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
-      <c r="L41" s="30"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="32"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="38"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="30"/>
+      <c r="A42" s="29"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="32"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="30"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="32"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="38"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="30"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="32"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="38"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="30"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="32"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
@@ -1538,8 +1550,8 @@
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
@@ -1552,7 +1564,7 @@
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
-      <c r="D48" s="18"/>
+      <c r="D48" s="16"/>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
@@ -1566,7 +1578,7 @@
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
-      <c r="D49" s="18"/>
+      <c r="D49" s="16"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
@@ -1580,7 +1592,7 @@
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
-      <c r="D50" s="18"/>
+      <c r="D50" s="16"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
@@ -1606,6 +1618,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="G23:L23"/>
+    <mergeCell ref="G12:L12"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="G14:L14"/>
+    <mergeCell ref="G15:L15"/>
+    <mergeCell ref="G16:L16"/>
+    <mergeCell ref="G17:L17"/>
+    <mergeCell ref="G18:L18"/>
+    <mergeCell ref="G19:L19"/>
+    <mergeCell ref="G20:L20"/>
+    <mergeCell ref="G21:L21"/>
+    <mergeCell ref="G22:L22"/>
+    <mergeCell ref="G35:L35"/>
+    <mergeCell ref="G24:L24"/>
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="G27:L27"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="G29:L29"/>
     <mergeCell ref="G42:L42"/>
     <mergeCell ref="G43:L43"/>
     <mergeCell ref="G44:L44"/>
@@ -1622,34 +1662,6 @@
     <mergeCell ref="G32:L32"/>
     <mergeCell ref="G33:L33"/>
     <mergeCell ref="G34:L34"/>
-    <mergeCell ref="G35:L35"/>
-    <mergeCell ref="G24:L24"/>
-    <mergeCell ref="G25:L25"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="G18:L18"/>
-    <mergeCell ref="G19:L19"/>
-    <mergeCell ref="G20:L20"/>
-    <mergeCell ref="G21:L21"/>
-    <mergeCell ref="G22:L22"/>
-    <mergeCell ref="G23:L23"/>
-    <mergeCell ref="G12:L12"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="G14:L14"/>
-    <mergeCell ref="G15:L15"/>
-    <mergeCell ref="G16:L16"/>
-    <mergeCell ref="G17:L17"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="G8:L8"/>
-    <mergeCell ref="G9:L9"/>
-    <mergeCell ref="G10:L10"/>
-    <mergeCell ref="G11:L11"/>
   </mergeCells>
   <conditionalFormatting sqref="B2">
     <cfRule type="expression" dxfId="0" priority="2">

</xml_diff>